<commit_message>
Added Images to make this fully functional
</commit_message>
<xml_diff>
--- a/Website Text.xlsx
+++ b/Website Text.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2e170692db1a7424/Documents/Tableau Projects/vizcatalogue/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="545" documentId="13_ncr:40001_{F0771C12-540E-4AA1-B0C2-D4D0F4ACD464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A20DC291-E430-49AC-A429-8F990BE5DEE3}"/>
+  <xr:revisionPtr revIDLastSave="547" documentId="13_ncr:40001_{F0771C12-540E-4AA1-B0C2-D4D0F4ACD464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{322AB046-F158-4B3C-8A38-04EA46C8F45D}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="301" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1705,8 +1705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L106" sqref="L106"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Updated the Hyperlink to open a new window
</commit_message>
<xml_diff>
--- a/Website Text.xlsx
+++ b/Website Text.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2e170692db1a7424/Documents/Tableau Projects/vizcatalogue/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="547" documentId="13_ncr:40001_{F0771C12-540E-4AA1-B0C2-D4D0F4ACD464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{322AB046-F158-4B3C-8A38-04EA46C8F45D}"/>
+  <xr:revisionPtr revIDLastSave="550" documentId="13_ncr:40001_{F0771C12-540E-4AA1-B0C2-D4D0F4ACD464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A02EA856-C1B3-4D08-A3C7-DBAC078499F5}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="301" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1705,8 +1705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:K1048576"/>
+    <sheetView tabSelected="1" topLeftCell="I98" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L103" sqref="L103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1715,10 +1715,10 @@
     <col min="2" max="3" width="47" style="1" customWidth="1"/>
     <col min="4" max="4" width="61" style="1" customWidth="1"/>
     <col min="5" max="6" width="9.1328125" style="1"/>
-    <col min="7" max="7" width="44.86328125" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="39.3984375" style="1" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="58.265625" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="34.3984375" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="44.86328125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="39.3984375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="58.265625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="34.3984375" style="1" customWidth="1"/>
     <col min="11" max="11" width="9.1328125" style="1"/>
     <col min="12" max="12" width="150.3984375" style="4" customWidth="1"/>
     <col min="13" max="16384" width="9.1328125" style="1"/>
@@ -1782,12 +1782,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Gauge Charts (With Arrow)&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Guage Chart (With Arrow) in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J2" s="1" t="str">
-        <f>"&lt;div class='card-action'&gt;&lt;a href='"&amp;D2&amp;"'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;"</f>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/gauge-chart-with-arrow/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <f>"&lt;div class='card-action'&gt;&lt;a target='_blank' href='"&amp;D2&amp;"'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;"</f>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/gauge-chart-with-arrow/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L2" s="5" t="str">
         <f>G2&amp;H2&amp;I2&amp;J2</f>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/gauge_chart_with_arrow.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Gauge Charts (With Arrow)&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Gauge Charts (With Arrow)&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Guage Chart (With Arrow) in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/gauge-chart-with-arrow/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/gauge_chart_with_arrow.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Gauge Charts (With Arrow)&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Gauge Charts (With Arrow)&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Guage Chart (With Arrow) in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/gauge-chart-with-arrow/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -1816,12 +1816,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Circular KPIs&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Circular KPIs in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J3" s="1" t="str">
-        <f t="shared" ref="J3:J65" si="3">"&lt;div class='card-action'&gt;&lt;a href='"&amp;D3&amp;"'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;"</f>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-circular-kpis-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <f t="shared" ref="J3:J66" si="3">"&lt;div class='card-action'&gt;&lt;a target='_blank' href='"&amp;D3&amp;"'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;"</f>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-circular-kpis-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L3" s="5" t="str">
         <f t="shared" ref="L3:L65" si="4">G3&amp;H3&amp;I3&amp;J3</f>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/circular_kpis.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Circular KPIs&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Circular KPIs&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Circular KPIs in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-circular-kpis-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/circular_kpis.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Circular KPIs&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Circular KPIs&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Circular KPIs in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-circular-kpis-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -1851,11 +1851,11 @@
       </c>
       <c r="J4" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-rounded-gantt-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-rounded-gantt-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L4" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/rounded_gantt_chart.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Rounded Gantt Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Rounded Gantt Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Rounded Gantt Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-rounded-gantt-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/rounded_gantt_chart.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Rounded Gantt Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Rounded Gantt Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Rounded Gantt Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-rounded-gantt-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -1885,11 +1885,11 @@
       </c>
       <c r="J5" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/single-level-sankey-diagram/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/single-level-sankey-diagram/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L5" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/single_level_sankey_chart.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Single Level Sankey Diagram&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Single Level Sankey Diagram&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Single Level Sankey Diagram in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/single-level-sankey-diagram/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/single_level_sankey_chart.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Single Level Sankey Diagram&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Single Level Sankey Diagram&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Single Level Sankey Diagram in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/single-level-sankey-diagram/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -1919,11 +1919,11 @@
       </c>
       <c r="J6" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-podium-bar-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-podium-bar-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L6" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/podium_chart.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Podium Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Podium Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Podium Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-podium-bar-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/podium_chart.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Podium Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Podium Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Podium Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-podium-bar-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -1953,11 +1953,11 @@
       </c>
       <c r="J7" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-curved-polar-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-curved-polar-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L7" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/curved_polar_chart.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Curved Polar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Curved Polar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Curved Polar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-curved-polar-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/curved_polar_chart.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Curved Polar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Curved Polar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Curved Polar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-curved-polar-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -1987,11 +1987,11 @@
       </c>
       <c r="J8" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-sketchy-bar-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-sketchy-bar-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L8" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/sketchy_bar_chart.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Sketchy Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Sketchy Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Sketchy Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-sketchy-bar-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/sketchy_bar_chart.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Sketchy Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Sketchy Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Sketchy Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-sketchy-bar-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -2021,11 +2021,11 @@
       </c>
       <c r="J9" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-a-polar-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-a-polar-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L9" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/polar_chart.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Polar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Polar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Polar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-a-polar-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/polar_chart.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Polar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Polar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Polar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-a-polar-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -2055,11 +2055,11 @@
       </c>
       <c r="J10" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-parallel-sets-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-parallel-sets-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L10" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/parallel_sets.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Parallel Sets&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Parallel Sets&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating Parallel Sets in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-parallel-sets-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/parallel_sets.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Parallel Sets&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Parallel Sets&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating Parallel Sets in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-parallel-sets-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -2089,11 +2089,11 @@
       </c>
       <c r="J11" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-win-loss-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-win-loss-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L11" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/win_loss_chart.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Win-Loss Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Win-Loss Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating Win-Loss Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-win-loss-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/win_loss_chart.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Win-Loss Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Win-Loss Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating Win-Loss Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-win-loss-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -2123,11 +2123,11 @@
       </c>
       <c r="J12" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/create-a-radial-column-chart-variation/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/create-a-radial-column-chart-variation/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L12" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/radial_column_chart_variation.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Radial Column Chart&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Radial Column Chart&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating Radial Column Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/create-a-radial-column-chart-variation/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/radial_column_chart_variation.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Radial Column Chart&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Radial Column Chart&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating Radial Column Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/create-a-radial-column-chart-variation/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -2157,11 +2157,11 @@
       </c>
       <c r="J13" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-a-bezier-curve-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-a-bezier-curve-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L13" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/bezier_curve.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Bezier Curve&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Bezier Curve&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Bezier Curve in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-a-bezier-curve-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/bezier_curve.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Bezier Curve&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Bezier Curve&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Bezier Curve in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-a-bezier-curve-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -2191,11 +2191,11 @@
       </c>
       <c r="J14" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-wilkinson-plot/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-wilkinson-plot/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L14" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/wilkinson_plot.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Wilkinson Plots&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Wilkinson Plots&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Wilkinson Plot in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-wilkinson-plot/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/wilkinson_plot.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Wilkinson Plots&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Wilkinson Plots&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Wilkinson Plot in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-wilkinson-plot/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -2225,11 +2225,11 @@
       </c>
       <c r="J15" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-tilted-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-tilted-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L15" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/tilted_bar_charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Tilted Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Tilted Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Tilted Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-tilted-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/tilted_bar_charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Tilted Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Tilted Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Tilted Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-tilted-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -2259,11 +2259,11 @@
       </c>
       <c r="J16" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-a-circular-network-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-a-circular-network-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L16" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/circular_network_chart.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Circular Network Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Circular Network Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Circular Network Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-a-circular-network-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/circular_network_chart.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Circular Network Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Circular Network Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Circular Network Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-a-circular-network-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -2293,11 +2293,11 @@
       </c>
       <c r="J17" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-jitter-stacked-bar-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-jitter-stacked-bar-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L17" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/jitter_stacked_bar_chart.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Jitter Stacked Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Jitter Stacked Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Jitter Stacked Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-jitter-stacked-bar-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/jitter_stacked_bar_chart.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Jitter Stacked Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Jitter Stacked Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Jitter Stacked Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-jitter-stacked-bar-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -2327,11 +2327,11 @@
       </c>
       <c r="J18" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-gradient-radial-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-gradient-radial-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L18" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/gradient_radial_bar_charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Gradient Radial Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Gradient Radial Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Gradient Radial Bar Charts in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-gradient-radial-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/gradient_radial_bar_charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Gradient Radial Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Gradient Radial Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Gradient Radial Bar Charts in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-gradient-radial-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -2361,11 +2361,11 @@
       </c>
       <c r="J19" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-negative-space-area-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-negative-space-area-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L19" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/negative_space_bar_chart.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Negative Space Area Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Negative Space Area Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Negative Space Area Charts in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-negative-space-area-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/negative_space_bar_chart.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Negative Space Area Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Negative Space Area Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Negative Space Area Charts in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-negative-space-area-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -2395,11 +2395,11 @@
       </c>
       <c r="J20" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-a-multi-level-dendrogram-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-a-multi-level-dendrogram-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L20" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/multi_level_dendrogram_charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Multi-Level Dendrogram Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Multi-Level Dendrogram Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Multi-Level Dendrogram Charts in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-a-multi-level-dendrogram-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/multi_level_dendrogram_charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Multi-Level Dendrogram Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Multi-Level Dendrogram Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Multi-Level Dendrogram Charts in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-a-multi-level-dendrogram-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -2429,11 +2429,11 @@
       </c>
       <c r="J21" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-half-circle-timelines-variation-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-half-circle-timelines-variation-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L21" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/half_circle_timeline_charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Half-Circle Timeline Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Half-Circle Timeline Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Half-Circle Timeline Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-half-circle-timelines-variation-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/half_circle_timeline_charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Half-Circle Timeline Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Half-Circle Timeline Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Half-Circle Timeline Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-half-circle-timelines-variation-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -2463,11 +2463,11 @@
       </c>
       <c r="J22" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-negative-space-bar-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-negative-space-bar-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L22" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/negative_space_bar_charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Negative Space Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Negative Space Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Negative Space Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-negative-space-bar-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/negative_space_bar_charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Negative Space Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Negative Space Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Negative Space Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-negative-space-bar-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -2497,11 +2497,11 @@
       </c>
       <c r="J23" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-a-spiral-stacked-line-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-a-spiral-stacked-line-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L23" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Spiral_Stacked_Line_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Spiral Stacked Line Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Spiral Stacked Line Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Spiral Stacked Line Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-a-spiral-stacked-line-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Spiral_Stacked_Line_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Spiral Stacked Line Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Spiral Stacked Line Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Spiral Stacked Line Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-a-spiral-stacked-line-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -2531,11 +2531,11 @@
       </c>
       <c r="J24" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-petal-polygon-diagrams/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-petal-polygon-diagrams/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L24" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Petal_Polygon_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Petal Polygon Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Petal Polygon Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Petal Polygon Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-petal-polygon-diagrams/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Petal_Polygon_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Petal Polygon Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Petal Polygon Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Petal Polygon Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-petal-polygon-diagrams/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -2565,11 +2565,11 @@
       </c>
       <c r="J25" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-floating-bar-charts-with-shaped-background/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-floating-bar-charts-with-shaped-background/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L25" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Floating_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Floating Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Floating Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a floating Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-floating-bar-charts-with-shaped-background/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Floating_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Floating Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Floating Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a floating Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-floating-bar-charts-with-shaped-background/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -2599,11 +2599,11 @@
       </c>
       <c r="J26" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-square-arc-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-square-arc-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L26" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Square_Arc_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Square Arc Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Square Arc Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Square Arc Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-square-arc-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Square_Arc_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Square Arc Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Square Arc Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Square Arc Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-square-arc-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -2633,11 +2633,11 @@
       </c>
       <c r="J27" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-curved-bar-chart-in-tableau-variation/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-curved-bar-chart-in-tableau-variation/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L27" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Curved_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Curved Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Curved Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Curved Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-curved-bar-chart-in-tableau-variation/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Curved_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Curved Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Curved Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Curved Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-curved-bar-chart-in-tableau-variation/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -2667,11 +2667,11 @@
       </c>
       <c r="J28" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-path-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-path-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L28" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Path_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Path Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Path Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Path Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-path-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Path_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Path Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Path Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Path Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-path-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -2701,11 +2701,11 @@
       </c>
       <c r="J29" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-step-line-chart-with-indicators/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-step-line-chart-with-indicators/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L29" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Step_Line_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Step Line Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Step Line Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Step Line Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-step-line-chart-with-indicators/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Step_Line_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Step Line Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Step Line Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Step Line Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-step-line-chart-with-indicators/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -2735,11 +2735,11 @@
       </c>
       <c r="J30" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-dendrogram-with-rounded-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-dendrogram-with-rounded-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L30" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Dendrogram_Charts_Rounded_Bars.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Dendrogram Charts (Rounded Bars)&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Dendrogram Charts (Rounded Bars)&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Denderogram with Rounded Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-dendrogram-with-rounded-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Dendrogram_Charts_Rounded_Bars.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Dendrogram Charts (Rounded Bars)&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Dendrogram Charts (Rounded Bars)&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Denderogram with Rounded Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-dendrogram-with-rounded-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -2769,11 +2769,11 @@
       </c>
       <c r="J31" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-squared-spiral-column-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-squared-spiral-column-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L31" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Squred_Spiral_Column_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Squred Spiral Column Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Squred Spiral Column Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Square Spiral Column Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-squared-spiral-column-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Squred_Spiral_Column_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Squred Spiral Column Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Squred Spiral Column Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Square Spiral Column Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-squared-spiral-column-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -2803,11 +2803,11 @@
       </c>
       <c r="J32" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-an-single-level-dendrogram-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-an-single-level-dendrogram-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L32" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Dendrogram_Charts_Single_Level.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Dendrogram Charts (Single Level)&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Dendrogram Charts (Single Level)&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Single Level Dendrogram Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-an-single-level-dendrogram-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Dendrogram_Charts_Single_Level.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Dendrogram Charts (Single Level)&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Dendrogram Charts (Single Level)&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Single Level Dendrogram Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-an-single-level-dendrogram-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -2837,11 +2837,11 @@
       </c>
       <c r="J33" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-variable-width-bar-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-variable-width-bar-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L33" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Variable_Width_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Variable Width Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Variable Width Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Variable Width Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-variable-width-bar-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Variable_Width_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Variable Width Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Variable Width Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Variable Width Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-variable-width-bar-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -2871,11 +2871,11 @@
       </c>
       <c r="J34" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-spiral-column-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-spiral-column-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L34" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Spiral_Column_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Spiral Column Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Spiral Column Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Spiral Column Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-spiral-column-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Spiral_Column_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Spiral Column Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Spiral Column Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Spiral Column Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-spiral-column-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -2905,11 +2905,11 @@
       </c>
       <c r="J35" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-nolan-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-nolan-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L35" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Nolan_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Nolan Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Nolan Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Nolan Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-nolan-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Nolan_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Nolan Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Nolan Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Nolan Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-nolan-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -2939,11 +2939,11 @@
       </c>
       <c r="J36" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-completion-gantt-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-completion-gantt-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L36" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Completion_Gantt_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Completion Gantt Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Completion Gantt Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Completion Gantt Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-completion-gantt-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Completion_Gantt_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Completion Gantt Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Completion Gantt Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Completion Gantt Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-completion-gantt-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -2973,11 +2973,11 @@
       </c>
       <c r="J37" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-square-bump-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-square-bump-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L37" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Square_Bump_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Square Bump Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Square Bump Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Square Bump Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-square-bump-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Square_Bump_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Square Bump Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Square Bump Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Square Bump Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-square-bump-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -3007,11 +3007,11 @@
       </c>
       <c r="J38" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-error-margin/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-error-margin/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L38" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Error_Margin_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Error Margin Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Error Margin Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating an Error Margin Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-error-margin/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Error_Margin_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Error Margin Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Error Margin Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating an Error Margin Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-error-margin/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -3041,11 +3041,11 @@
       </c>
       <c r="J39" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-radial-jitter-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-radial-jitter-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L39" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Radial_Jitter_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Radial Jitter Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Radial Jitter Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Radial Jitter Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-radial-jitter-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Radial_Jitter_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Radial Jitter Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Radial Jitter Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Radial Jitter Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-radial-jitter-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -3075,11 +3075,11 @@
       </c>
       <c r="J40" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-rootogram/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-rootogram/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L40" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Rootogram.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Rootogram&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Rootogram&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Rootogram Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-rootogram/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Rootogram.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Rootogram&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Rootogram&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Rootogram Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-rootogram/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -3109,11 +3109,11 @@
       </c>
       <c r="J41" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/create-a-bar-chart-textured-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/create-a-bar-chart-textured-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L41" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Textured_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Textured Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Textured Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Textured Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/create-a-bar-chart-textured-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Textured_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Textured Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Textured Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Textured Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/create-a-bar-chart-textured-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -3143,11 +3143,11 @@
       </c>
       <c r="J42" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-histogram-with-normal-curve/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-histogram-with-normal-curve/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L42" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Histogram_with_Normal_Curve.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Histogram with Normal Curve&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Histogram with Normal Curve&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Histogram with Normal Curve in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-histogram-with-normal-curve/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Histogram_with_Normal_Curve.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Histogram with Normal Curve&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Histogram with Normal Curve&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Histogram with Normal Curve in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-histogram-with-normal-curve/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -3177,11 +3177,11 @@
       </c>
       <c r="J43" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-a-gradient-pie-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-a-gradient-pie-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L43" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Gradient_Pie_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Gradient Pie Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Gradient Pie Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Gradient Pie Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-a-gradient-pie-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Gradient_Pie_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Gradient Pie Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Gradient Pie Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Gradient Pie Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-a-gradient-pie-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -3211,11 +3211,11 @@
       </c>
       <c r="J44" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-ohlc-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-ohlc-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L44" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/OHLC_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;OHLC Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;OHLC Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Open-High-Low-Close Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-ohlc-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/OHLC_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;OHLC Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;OHLC Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Open-High-Low-Close Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-ohlc-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -3245,11 +3245,11 @@
       </c>
       <c r="J45" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/shaped-bar-charts-3d-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/shaped-bar-charts-3d-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L45" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/3D_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;3D Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;3D Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a 3D Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/shaped-bar-charts-3d-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/3D_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;3D Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;3D Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a 3D Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/shaped-bar-charts-3d-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -3279,11 +3279,11 @@
       </c>
       <c r="J46" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-a-marimekko-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-a-marimekko-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L46" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Marrimekko_Chart.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Marrimekko Chart&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Marrimekko Chart&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Marrimekko Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-a-marimekko-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Marrimekko_Chart.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Marrimekko Chart&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Marrimekko Chart&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Marrimekko Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-a-marimekko-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -3313,11 +3313,11 @@
       </c>
       <c r="J47" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-a-pudding-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-a-pudding-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L47" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Pudding_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Pudding Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Pudding Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Pudding Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-a-pudding-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Pudding_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Pudding Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Pudding Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Pudding Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-a-pudding-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -3347,11 +3347,11 @@
       </c>
       <c r="J48" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-bar-chart-with-floating-icons/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-bar-chart-with-floating-icons/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L48" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Floating_Icon_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Floating Icon Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Floating Icon Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Floating Icon Bar Charts in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-bar-chart-with-floating-icons/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Floating_Icon_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Floating Icon Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Floating Icon Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Floating Icon Bar Charts in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-bar-chart-with-floating-icons/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -3381,11 +3381,11 @@
       </c>
       <c r="J49" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-radial-column-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-radial-column-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L49" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Radial_Column_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Radial Column Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Radial Column Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Radial Column Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-radial-column-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Radial_Column_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Radial Column Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Radial Column Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Radial Column Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-radial-column-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -3415,11 +3415,11 @@
       </c>
       <c r="J50" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-a-coxcomb-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-a-coxcomb-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L50" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Coxcomb_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Coxcomb Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Coxcomb Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Coxcomb Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-a-coxcomb-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Coxcomb_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Coxcomb Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Coxcomb Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Coxcomb Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-a-coxcomb-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -3449,11 +3449,11 @@
       </c>
       <c r="J51" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-gradient-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-gradient-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L51" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Gradient_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Gradient Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Gradient Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Gradient Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-gradient-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Gradient_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Gradient Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Gradient Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Gradient Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-gradient-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -3483,11 +3483,11 @@
       </c>
       <c r="J52" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-radial-stacked-bar-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-radial-stacked-bar-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L52" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Radial_Stacked_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Radial Stacked Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Radial Stacked Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Radial Stacked Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-radial-stacked-bar-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Radial_Stacked_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Radial Stacked Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Radial Stacked Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Radial Stacked Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-radial-stacked-bar-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -3517,11 +3517,11 @@
       </c>
       <c r="J53" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-quadrant-plots/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-quadrant-plots/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L53" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Quadrant_Plots.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Quadrant Plots&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Quadrant Plots&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Quadrant Plot in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-quadrant-plots/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Quadrant_Plots.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Quadrant Plots&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Quadrant Plots&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Quadrant Plot in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-quadrant-plots/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -3551,11 +3551,11 @@
       </c>
       <c r="J54" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-bar-with-trend-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-bar-with-trend-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L54" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Bar_with_Trend_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Bar with Trend Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Bar with Trend Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Bar with Trend Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-bar-with-trend-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Bar_with_Trend_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Bar with Trend Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Bar with Trend Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Bar with Trend Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-bar-with-trend-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -3585,11 +3585,11 @@
       </c>
       <c r="J55" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-gauges-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-gauges-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L55" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Gauge_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Gauge Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Gauge Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Gauge Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-gauges-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Gauge_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Gauge Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Gauge Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Gauge Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-gauges-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -3619,11 +3619,11 @@
       </c>
       <c r="J56" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-volume-dial-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-volume-dial-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L56" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Volume_Dial_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Volume Dial Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Volume Dial Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Volume Dial Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-volume-dial-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Volume_Dial_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Volume Dial Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Volume Dial Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Volume Dial Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-volume-dial-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -3653,11 +3653,11 @@
       </c>
       <c r="J57" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-half-circle-gauge-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-half-circle-gauge-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L57" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Half_Circle_Gauge_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Half-Circle Gauge Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Half-Circle Gauge Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Half-Circle Gauge Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-half-circle-gauge-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Half_Circle_Gauge_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Half-Circle Gauge Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Half-Circle Gauge Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Half-Circle Gauge Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-half-circle-gauge-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -3687,11 +3687,11 @@
       </c>
       <c r="J58" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-calendar-circle-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-calendar-circle-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L58" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Calendar_Circle_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Calendar Circle Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Calendar Circle Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Calendar Circle Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-calendar-circle-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Calendar_Circle_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Calendar Circle Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Calendar Circle Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Calendar Circle Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-calendar-circle-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -3721,11 +3721,11 @@
       </c>
       <c r="J59" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-rounded-stacked-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-rounded-stacked-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L59" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Rounded_Stacked_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Rounded Stacked Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Rounded Stacked Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Rounded Stacked Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-rounded-stacked-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Rounded_Stacked_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Rounded Stacked Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Rounded Stacked Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Rounded Stacked Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-rounded-stacked-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="60" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -3755,11 +3755,11 @@
       </c>
       <c r="J60" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-layered-area-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-layered-area-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L60" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Layered_Area_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Layered Area Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Layered Area Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Layered Area Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-layered-area-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Layered_Area_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Layered Area Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Layered Area Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Layered Area Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-layered-area-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="61" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -3789,11 +3789,11 @@
       </c>
       <c r="J61" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-jitter-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-jitter-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L61" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Jitter_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Jitter Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Jitter Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Jitter Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-jitter-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Jitter_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Jitter Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Jitter Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Jitter Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-jitter-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="62" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -3823,11 +3823,11 @@
       </c>
       <c r="J62" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-spiral-hex-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-spiral-hex-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L62" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Spiral_Hex_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Spiral Hex Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Spiral Hex Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Spiral Hex Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-spiral-hex-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Spiral_Hex_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Spiral Hex Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Spiral Hex Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Spiral Hex Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-spiral-hex-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="63" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -3857,11 +3857,11 @@
       </c>
       <c r="J63" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-square-area-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-square-area-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L63" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Square_Area_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Square Area Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Square Area Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Square Area Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-square-area-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Square_Area_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Square Area Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Square Area Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Square Area Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-square-area-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="64" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -3891,11 +3891,11 @@
       </c>
       <c r="J64" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/drawing-neon-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/drawing-neon-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L64" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Neon_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Neon Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Neon Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Neon Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/drawing-neon-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Neon_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Neon Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Neon Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Neon Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/drawing-neon-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="65" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -3925,11 +3925,11 @@
       </c>
       <c r="J65" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/drawing-layered-filled-circle-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/drawing-layered-filled-circle-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L65" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Layered_Filled_Circle_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Layered Filled Circle Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Layered Filled Circle Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Layered Filled Circle Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/drawing-layered-filled-circle-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Layered_Filled_Circle_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Layered Filled Circle Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Layered Filled Circle Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Layered Filled Circle Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/drawing-layered-filled-circle-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="66" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -3958,12 +3958,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Ternary Plots&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Ternary Plot in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J66" s="1" t="str">
-        <f t="shared" ref="J66:J106" si="8">"&lt;div class='card-action'&gt;&lt;a href='"&amp;D66&amp;"'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;"</f>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-ternary-plots-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <f t="shared" si="3"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-ternary-plots-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
       <c r="L66" s="5" t="str">
-        <f t="shared" ref="L66:L106" si="9">G66&amp;H66&amp;I66&amp;J66</f>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Ternary_Plots.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Ternary Plots&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Ternary Plots&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Ternary Plot in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/creating-ternary-plots-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <f t="shared" ref="L66:L106" si="8">G66&amp;H66&amp;I66&amp;J66</f>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Ternary_Plots.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Ternary Plots&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Ternary Plots&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Ternary Plot in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/creating-ternary-plots-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="67" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -3992,12 +3992,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Tally Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Tally Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J67" s="1" t="str">
+        <f t="shared" ref="J67:J106" si="9">"&lt;div class='card-action'&gt;&lt;a target='_blank' href='"&amp;D67&amp;"'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;"</f>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/drawing-tally-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L67" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/drawing-tally-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L67" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Tally_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Tally Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Tally Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Tally Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/drawing-tally-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Tally_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Tally Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Tally Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Tally Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/drawing-tally-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="68" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -4026,12 +4026,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Curved Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating Curved Bar Charts in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J68" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/drawing-curved-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L68" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/drawing-curved-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L68" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Curved_Bar_Charts2.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Curved Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Curved Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating Curved Bar Charts in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/drawing-curved-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Curved_Bar_Charts2.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Curved Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Curved Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating Curved Bar Charts in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/drawing-curved-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="69" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -4060,12 +4060,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Triangle Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Triangle Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J69" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/drawing-triangle-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L69" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/drawing-triangle-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L69" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Triangle_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Triangle Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Triangle Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Triangle Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/drawing-triangle-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Triangle_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Triangle Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Triangle Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Triangle Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/drawing-triangle-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="70" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -4094,12 +4094,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Candlestick Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Candlestick Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J70" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/drawing-candlestick-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L70" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/drawing-candlestick-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L70" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Candlestick_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Candlestick Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Candlestick Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Candlestick Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/drawing-candlestick-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Candlestick_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Candlestick Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Candlestick Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Candlestick Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/drawing-candlestick-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="71" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -4128,12 +4128,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Hex Maps&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Hex Map in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J71" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/hex-maps-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L71" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/hex-maps-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L71" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Hex_Maps.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Hex Maps&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Hex Maps&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Hex Map in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/hex-maps-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Hex_Maps.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Hex Maps&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Hex Maps&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Hex Map in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/hex-maps-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="72" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -4162,12 +4162,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Sigmoid Area Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Sigmoid Area Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J72" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/sigmoid-area-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L72" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/sigmoid-area-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L72" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Sigmoid_Area_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Sigmoid Area Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Sigmoid Area Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Sigmoid Area Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/sigmoid-area-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Sigmoid_Area_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Sigmoid Area Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Sigmoid Area Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Sigmoid Area Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/sigmoid-area-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="73" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -4196,12 +4196,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Connected Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Connected Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J73" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-connected-bar-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L73" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-connected-bar-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L73" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Connected_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Connected Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Connected Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Connected Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-connected-bar-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Connected_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Connected Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Connected Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Connected Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-connected-bar-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="74" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -4230,12 +4230,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Spiral Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Spiral Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J74" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-spiral-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L74" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-spiral-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L74" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Spiral_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Spiral Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Spiral Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Spiral Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-spiral-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Spiral_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Spiral Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Spiral Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Spiral Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-spiral-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="75" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -4264,12 +4264,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Arrow Doughnut Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Arrow Doughnut Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J75" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/arrow-doughnut-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L75" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/arrow-doughnut-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L75" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Arrow_Doughnut_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Arrow Doughnut Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Arrow Doughnut Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Arrow Doughnut Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/arrow-doughnut-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Arrow_Doughnut_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Arrow Doughnut Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Arrow Doughnut Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Arrow Doughnut Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/arrow-doughnut-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="76" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -4298,12 +4298,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Cylinder Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Cylinder Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J76" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/cylinder-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L76" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/cylinder-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L76" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Cylinder_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Cylinder Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Cylinder Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Cylinder Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/cylinder-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Cylinder_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Cylinder Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Cylinder Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Cylinder Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/cylinder-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="77" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -4332,12 +4332,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Waffle Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Waffle Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J77" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/waffle-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L77" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/waffle-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L77" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Waffle_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Waffle Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Waffle Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Waffle Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/waffle-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Waffle_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Waffle Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Waffle Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Waffle Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/waffle-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="78" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -4366,12 +4366,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Circular Jitter Plots&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Circular Jitter Plot in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J78" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/circular-jitter-plots-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L78" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/circular-jitter-plots-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L78" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Circular_Jitter_Plots.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Circular Jitter Plots&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Circular Jitter Plots&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Circular Jitter Plot in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/circular-jitter-plots-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Circular_Jitter_Plots.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Circular Jitter Plots&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Circular Jitter Plots&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Circular Jitter Plot in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/circular-jitter-plots-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="79" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -4400,12 +4400,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Filled Circle Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Filled Circle Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J79" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/filled-circle-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L79" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/filled-circle-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L79" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Filled_Circle_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Filled Circle Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Filled Circle Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Filled Circle Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/filled-circle-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Filled_Circle_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Filled Circle Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Filled Circle Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Filled Circle Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/filled-circle-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="80" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -4434,12 +4434,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Dot Quadrant Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Dot Quadrant Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J80" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/dot-quadrant-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L80" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/dot-quadrant-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L80" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Dot_Quadrant_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Dot Quadrant Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Dot Quadrant Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Dot Quadrant Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/dot-quadrant-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Dot_Quadrant_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Dot Quadrant Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Dot Quadrant Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Dot Quadrant Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/dot-quadrant-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="81" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -4468,12 +4468,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Pyramid Step Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Pyramid Step Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J81" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-pyramid-step-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L81" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-pyramid-step-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L81" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Pyramid_Step_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Pyramid Step Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Pyramid Step Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Pyramid Step Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-pyramid-step-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Pyramid_Step_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Pyramid Step Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Pyramid Step Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Pyramid Step Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-pyramid-step-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="82" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -4502,12 +4502,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Thermometer Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Thermometer Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J82" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-thermometer-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L82" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-thermometer-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L82" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Thermometer_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Thermometer Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Thermometer Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Thermometer Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-thermometer-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Thermometer_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Thermometer Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Thermometer Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Thermometer Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-thermometer-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="83" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -4536,12 +4536,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Circle Dot Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Circle Dot Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J83" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/drawing-a-circle-dot-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L83" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/drawing-a-circle-dot-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L83" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Circle_Dot_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Circle Dot Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Circle Dot Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Circle Dot Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/drawing-a-circle-dot-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Circle_Dot_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Circle Dot Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Circle Dot Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Circle Dot Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/drawing-a-circle-dot-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="84" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -4570,12 +4570,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Waterfall Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Waterfall Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J84" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-waterfall-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L84" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-waterfall-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L84" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Waterfall_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Waterfall Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Waterfall Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Waterfall Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-waterfall-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Waterfall_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Waterfall Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Waterfall Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Waterfall Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-waterfall-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="85" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -4604,12 +4604,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Shaped Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Shaped Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J85" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-shape-bar-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L85" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-shape-bar-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L85" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Shaped_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Shaped Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Shaped Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Shaped Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-shape-bar-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Shaped_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Shaped Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Shaped Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Shaped Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-shape-bar-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="86" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -4638,12 +4638,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Radial Fan Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Radial Fan Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J86" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/radial-fan-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L86" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/radial-fan-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L86" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Radial_Fan_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Radial Fan Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Radial Fan Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Radial Fan Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/radial-fan-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Radial_Fan_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Radial Fan Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Radial Fan Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Radial Fan Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/radial-fan-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="87" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -4672,12 +4672,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Daisy Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Daisy Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J87" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/drawing-daisy-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L87" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/drawing-daisy-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L87" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Daisy_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Daisy Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Daisy Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Daisy Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/drawing-daisy-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Daisy_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Daisy Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Daisy Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Daisy Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/drawing-daisy-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="88" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -4706,12 +4706,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Connected Weighted Bump Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Connected Weighted Bump Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J88" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-magic-epicviz-vol-1/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L88" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-magic-epicviz-vol-1/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L88" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Epic_Viz.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Connected Weighted Bump Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Connected Weighted Bump Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Connected Weighted Bump Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-magic-epicviz-vol-1/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Epic_Viz.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Connected Weighted Bump Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Connected Weighted Bump Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Connected Weighted Bump Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-magic-epicviz-vol-1/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="89" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -4740,12 +4740,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Sin-Dumbbell Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Sin-Dumbbell Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J89" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-sin-dumbbell-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L89" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-sin-dumbbell-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L89" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Sin_Dumbbell_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Sin-Dumbbell Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Sin-Dumbbell Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Sin-Dumbbell Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-sin-dumbbell-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Sin_Dumbbell_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Sin-Dumbbell Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Sin-Dumbbell Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Sin-Dumbbell Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-sin-dumbbell-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="90" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -4774,12 +4774,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Radial Rounded Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Combined Radial and Rounded Bar Charts in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J90" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/drawing-a-combined-radial-and-rounded-bar-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L90" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/drawing-a-combined-radial-and-rounded-bar-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L90" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Radial_Rounded_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Radial Rounded Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Radial Rounded Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Combined Radial and Rounded Bar Charts in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/drawing-a-combined-radial-and-rounded-bar-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Radial_Rounded_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Radial Rounded Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Radial Rounded Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Combined Radial and Rounded Bar Charts in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/drawing-a-combined-radial-and-rounded-bar-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="91" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -4808,12 +4808,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Bump Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Bump Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J91" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-league-table/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L91" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-league-table/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L91" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Bump_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Bump Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Bump Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Bump Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-league-table/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Bump_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Bump Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Bump Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Bump Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-league-table/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="92" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -4842,12 +4842,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Rounded Doughnut Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Rounded Doughnut Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J92" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-rounded-doughnut-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L92" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-rounded-doughnut-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L92" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Rounded_Doughnut_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Rounded Doughnut Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Rounded Doughnut Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Rounded Doughnut Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-rounded-doughnut-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Rounded_Doughnut_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Rounded Doughnut Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Rounded Doughnut Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Rounded Doughnut Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-rounded-doughnut-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="93" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -4876,12 +4876,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Funnel Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Funnel Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J93" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-funnel-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L93" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-funnel-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L93" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Funnel_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Funnel Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Funnel Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Funnel Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-funnel-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Funnel_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Funnel Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Funnel Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Funnel Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-funnel-chart/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="94" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -4910,12 +4910,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Drop-Off Sankey Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Dropoff Sankey Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J94" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/drawing-a-drop-off-sankey-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L94" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/drawing-a-drop-off-sankey-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L94" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Drop_Off_Sankey_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Drop-Off Sankey Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Drop-Off Sankey Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Dropoff Sankey Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/drawing-a-drop-off-sankey-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Drop_Off_Sankey_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Drop-Off Sankey Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Drop-Off Sankey Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Dropoff Sankey Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/drawing-a-drop-off-sankey-chart-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="95" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -4944,12 +4944,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Square Radial Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Square Radial Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J95" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/drawing-square-radial-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L95" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/drawing-square-radial-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L95" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Square_Radial_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Square Radial Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Square Radial Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Square Radial Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/drawing-square-radial-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Square_Radial_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Square Radial Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Square Radial Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Square Radial Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/drawing-square-radial-bar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="96" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -4978,12 +4978,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Radar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Radar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J96" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/drawing-radar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L96" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/drawing-radar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L96" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Radar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Radar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Radar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Radar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/drawing-radar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Radar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Radar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Radar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Radar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/drawing-radar-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="97" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -5012,12 +5012,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Curved Line Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Curved Line Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J97" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-curved-lines/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L97" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-curved-lines/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L97" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Curved_Line_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Curved Line Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Curved Line Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Curved Line Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-curved-lines/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Curved_Line_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Curved Line Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Curved Line Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Curved Line Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-curved-lines/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="98" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -5046,12 +5046,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Petal Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Petal Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J98" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/petal-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L98" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/petal-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L98" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Petal_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Petal Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Petal Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Petal Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/petal-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Petal_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Petal Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Petal Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Petal Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/petal-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="99" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -5080,12 +5080,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Half-Circle Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Half-Circle Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J99" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/half-circle-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L99" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/half-circle-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L99" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Half_Circle_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Half-Circle Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Half-Circle Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Half-Circle Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/half-circle-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Half_Circle_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Half-Circle Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Half-Circle Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Half-Circle Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/half-circle-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="100" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -5114,12 +5114,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Rounded Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Rounded Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J100" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-rounded-bar-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L100" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-rounded-bar-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L100" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Rounded_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Rounded Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Rounded Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Rounded Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/tableau-qt-rounded-bar-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Rounded_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Rounded Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Rounded Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Rounded Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/tableau-qt-rounded-bar-charts/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="101" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -5148,12 +5148,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Venn Diagrams&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Venn Diagram in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J101" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/venn-diagrams-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L101" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/venn-diagrams-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L101" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Venn_Diagrams.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Venn Diagrams&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Venn Diagrams&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Venn Diagram in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/venn-diagrams-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Venn_Diagrams.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Venn Diagrams&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Venn Diagrams&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Venn Diagram in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/venn-diagrams-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="102" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -5182,12 +5182,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Packed Circle Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Packed Circle Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J102" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/packed-circle-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L102" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/packed-circle-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L102" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Packed_Circle_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Packed Circle Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Packed Circle Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Packed Circle Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/packed-circle-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Packed_Circle_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Packed Circle Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Packed Circle Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Packed Circle Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/packed-circle-charts-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="103" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -5216,12 +5216,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Process Circles&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Process Circle in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J103" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/drawing-process-circles-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L103" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/drawing-process-circles-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L103" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Process_Circles.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Process Circles&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Process Circles&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Process Circle in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/drawing-process-circles-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Process_Circles.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Process Circles&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Process Circles&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Process Circle in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/drawing-process-circles-in-tableau/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="104" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -5250,12 +5250,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Radial Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Radial Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J104" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/radial-bar-chart-tutorial/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L104" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/radial-bar-chart-tutorial/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L104" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Radial_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Radial Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Radial Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Radial Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/radial-bar-chart-tutorial/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Radial_Bar_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Radial Bar Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Radial Bar Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Radial Bar Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/radial-bar-chart-tutorial/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="105" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -5284,12 +5284,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Dual-Metric Doughnut Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Dual Metric Doughnut Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J105" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/dual-metric-doughnut-chart-tutorial/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L105" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/dual-metric-doughnut-chart-tutorial/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L105" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Dual_Metric_Doughnut_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Dual-Metric Doughnut Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Dual-Metric Doughnut Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Dual Metric Doughnut Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/dual-metric-doughnut-chart-tutorial/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Dual_Metric_Doughnut_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Dual-Metric Doughnut Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Dual-Metric Doughnut Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Dual Metric Doughnut Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/dual-metric-doughnut-chart-tutorial/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="106" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
@@ -5318,12 +5318,12 @@
         <v>&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Sunburst Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Sunburst Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</v>
       </c>
       <c r="J106" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/sunburst-chart-tutorial/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+      <c r="L106" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/sunburst-chart-tutorial/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
-      </c>
-      <c r="L106" s="5" t="str">
-        <f t="shared" si="9"/>
-        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Sunburst_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Sunburst Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Sunburst Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Sunburst Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a href='https://tableau.toanhoang.com/sunburst-chart-tutorial/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
+        <v>&lt;div class='col s12 m6 l4'&gt;&lt;div class='card sticky-action'&gt;&lt;div class='card-image waves-effect waves-block waves-light'&gt;&lt;img class='activator' src='img/Sunburst_Charts.png'/&gt;&lt;/div&gt;&lt;div class='card-content'&gt;&lt;span class='card-title activator grey-text text-darken-4'&gt;&lt;span class='card-search'&gt;Sunburst Charts&lt;/span&gt;&lt;i class='material-icons right'&gt;more_vert&lt;/i&gt;&lt;/span&gt;&lt;/div&gt;&lt;div class='card-reveal'&gt;&lt;span class='card-title grey-text text-darken-4'&gt;Sunburst Charts&lt;i class='material-icons right'&gt;close&lt;/i&gt;&lt;/span&gt;&lt;p&gt;Creating a Sunburst Chart in Tableau&lt;/p&gt;&lt;p&gt;&lt;/p&gt;&lt;div class='card-action'&gt;&lt;a target='_blank' href='https://tableau.toanhoang.com/sunburst-chart-tutorial/'&gt;View Tutorial&lt;/a&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.45">

</xml_diff>